<commit_message>
ACO routing relevant input
</commit_message>
<xml_diff>
--- a/Input data/Graph.xlsx
+++ b/Input data/Graph.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lichen/PycharmProjects/ACO_Example/Input data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23AC9DDA-A9BC-0141-B459-68F769C98774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78BB8E64-AE5B-564B-A650-3DE97B5F7F33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="500" windowWidth="27580" windowHeight="16940" xr2:uid="{B444C7B0-2106-E747-B393-7077F39B6589}"/>
+    <workbookView xWindow="1220" yWindow="500" windowWidth="27580" windowHeight="15800" activeTab="1" xr2:uid="{B444C7B0-2106-E747-B393-7077F39B6589}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -23,9 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>Cost</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -45,6 +44,10 @@
   </si>
   <si>
     <t>Node2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Distance</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -411,8 +414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A550BFA5-52EE-9242-9988-46359F551493}">
   <dimension ref="A1:C162"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2514,4 +2517,334 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F67373B1-F0BC-2C45-BDC5-3BCACC4126DB}">
+  <dimension ref="A1:C29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>6</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>7</v>
+      </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27">
+        <v>15</v>
+      </c>
+      <c r="B27">
+        <v>21</v>
+      </c>
+      <c r="C27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28">
+        <v>16</v>
+      </c>
+      <c r="B28">
+        <v>17</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="C29">
+        <f>SUM(C2:C28)</f>
+        <v>316</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>